<commit_message>
feat: 1.1.0 添加compare_avl_sheets函数,用于对比AVL和AVL_Cmp两个sheet的数据 程序由AI生成
</commit_message>
<xml_diff>
--- a/third_party/Excel_Handle/AVL_Cmp_Same_List_Example.xlsx
+++ b/third_party/Excel_Handle/AVL_Cmp_Same_List_Example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://abb-my.sharepoint.com/personal/mackey-jinhuan_lao_cn_abb_com/Documents/00_WorkPlace/01_Design_Work/01_Prg/10_Py/PythonCode/A1_Flask/Flask_CONNECT_DB/third_party/Excel_Handle/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{DAAC8FC7-9078-4B7B-AE10-9F02F9836504}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C61A99C7-BA84-47C4-9416-09A4C13A1DBF}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:1_{DAAC8FC7-9078-4B7B-AE10-9F02F9836504}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7CF12A2C-0088-47BB-8154-64C9CD1361AF}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8940" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AVL" sheetId="1" r:id="rId1"/>
@@ -26,8 +26,77 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Mackey-JinHuan Lao</author>
+  </authors>
+  <commentList>
+    <comment ref="B50" authorId="0" shapeId="0" xr:uid="{05E60AD0-D87C-4045-96FE-3BFF03E30E31}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Mackey-JinHuan Lao:for </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>New part test
+2TFU901483U1001</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Mackey-JinHuan Lao</author>
+  </authors>
+  <commentList>
+    <comment ref="B54" authorId="0" shapeId="0" xr:uid="{8F4DB393-14F8-409E-BD44-AA7BE82484B9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Mackey-JinHuan Lao:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+for delete part test
+2TFU901320U1001</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="265">
   <si>
     <t xml:space="preserve">ABB </t>
   </si>
@@ -828,7 +897,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -909,6 +978,19 @@
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1426,14 +1508,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:T54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K45" sqref="K45"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="1"/>
@@ -2300,7 +2382,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:3">
       <c r="A49">
         <v>43</v>
       </c>
@@ -2311,30 +2393,8 @@
         <v>152</v>
       </c>
     </row>
-    <row r="50" spans="1:8">
-      <c r="A50">
-        <v>44</v>
-      </c>
-      <c r="B50" t="s">
-        <v>153</v>
-      </c>
-      <c r="C50" t="s">
-        <v>154</v>
-      </c>
-      <c r="E50" t="s">
-        <v>29</v>
-      </c>
-      <c r="F50" t="s">
-        <v>155</v>
-      </c>
-      <c r="G50" t="s">
-        <v>31</v>
-      </c>
-      <c r="H50" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8">
+    <row r="50" spans="1:3"/>
+    <row r="51" spans="1:3">
       <c r="A51">
         <v>45</v>
       </c>
@@ -2345,7 +2405,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:3">
       <c r="A52">
         <v>46</v>
       </c>
@@ -2356,7 +2416,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:3">
       <c r="A53">
         <v>47</v>
       </c>
@@ -2367,7 +2427,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:3">
       <c r="A54">
         <v>48</v>
       </c>
@@ -2388,18 +2448,19 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FD83B7A-67B6-4C15-B32B-ED94D88A7750}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FD83B7A-67B6-4C15-B32B-ED94D88A7750}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:T54"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O41" sqref="O41"/>
+    <sheetView topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="1"/>
@@ -3729,29 +3790,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="54" spans="1:8">
-      <c r="A54">
-        <v>48</v>
-      </c>
-      <c r="B54" t="s">
-        <v>80</v>
-      </c>
-      <c r="C54" t="s">
-        <v>81</v>
-      </c>
-      <c r="E54" t="s">
-        <v>29</v>
-      </c>
-      <c r="F54" t="s">
-        <v>82</v>
-      </c>
-      <c r="G54" t="s">
-        <v>31</v>
-      </c>
-      <c r="H54" t="s">
-        <v>83</v>
-      </c>
-    </row>
+    <row r="54" spans="1:8"/>
   </sheetData>
   <autoFilter ref="A6:S7" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="4">
@@ -3762,6 +3801,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
feat: AVL_Excel_Handle中增加get_SAP_Numbers_from_AVL_sheet()函数, 用于获取AVL表中的Part列表 版本1.3.0 之前的修改忘记升版和添加log
</commit_message>
<xml_diff>
--- a/third_party/Excel_Handle/AVL_Cmp_Same_List_Example.xlsx
+++ b/third_party/Excel_Handle/AVL_Cmp_Same_List_Example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://abb-my.sharepoint.com/personal/mackey-jinhuan_lao_cn_abb_com/Documents/00_WorkPlace/01_Design_Work/01_Prg/10_Py/PythonCode/A1_Flask/Flask_CONNECT_DB/third_party/Excel_Handle/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="13_ncr:1_{DAAC8FC7-9078-4B7B-AE10-9F02F9836504}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B51F8DA5-3031-4156-B162-E6856B4B7420}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="13_ncr:1_{DAAC8FC7-9078-4B7B-AE10-9F02F9836504}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E86380A9-BFC2-4F14-B773-87A70E468739}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25320" yWindow="-4905" windowWidth="25440" windowHeight="15270" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AVL" sheetId="1" r:id="rId1"/>
@@ -96,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="267">
   <si>
     <t xml:space="preserve">ABB </t>
   </si>
@@ -891,13 +891,19 @@
   </si>
   <si>
     <t>CC0805KRX7R7BB47*</t>
+  </si>
+  <si>
+    <t>2TFE001021D1802</t>
+  </si>
+  <si>
+    <t>2TFE001021D1803</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -991,6 +997,13 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -2463,7 +2476,7 @@
   </sheetPr>
   <dimension ref="A1:T54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
@@ -3818,8 +3831,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B2:C494"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -3848,11 +3861,12 @@
       </c>
     </row>
     <row r="4" spans="2:3">
-      <c r="B4" s="13"/>
+      <c r="B4" s="13" t="s">
+        <v>265</v>
+      </c>
       <c r="C4" s="13"/>
     </row>
     <row r="5" spans="2:3">
-      <c r="B5" s="13"/>
       <c r="C5" s="13"/>
     </row>
     <row r="6" spans="2:3">
@@ -3860,7 +3874,9 @@
       <c r="C6" s="13"/>
     </row>
     <row r="7" spans="2:3">
-      <c r="B7" s="13"/>
+      <c r="B7" s="13" t="s">
+        <v>266</v>
+      </c>
       <c r="C7" s="13"/>
     </row>
     <row r="8" spans="2:3">
@@ -5812,6 +5828,7 @@
       <c r="C494" s="13"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="14" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0"/>
 </worksheet>

</xml_diff>